<commit_message>
Update project template with the package containing AutoReceiptActivity.
</commit_message>
<xml_diff>
--- a/templates/CcintOcrBasicProcess/config/recognizer_config.xlsx
+++ b/templates/CcintOcrBasicProcess/config/recognizer_config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\allenlooplee\Documents\GitHub\CcintOcrActivitiesPack\tests\CcintOcrBasicTests\Tests_Data\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54505FFF-D84C-4CF6-A4C4-3B1C168E275B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38389BE4-F952-4DB0-AE32-ED1F4022518E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="18436" windowHeight="11160" xr2:uid="{D6D768DA-5964-4C9E-A98A-0598DDF1AEA9}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>AppKey</t>
   </si>
@@ -69,6 +69,12 @@
   </si>
   <si>
     <t>https://ocr-api.ccint.com/cci_ai/service/v1/id_card</t>
+  </si>
+  <si>
+    <t>auto_receipt</t>
+  </si>
+  <si>
+    <t>https://ocr-api.ccint.com/cci_ai/service/v1/general_receipt_recog</t>
   </si>
 </sst>
 </file>
@@ -432,16 +438,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41493430-721B-460C-97F1-874FC5931AF2}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="C6" sqref="C6:D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="48.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53.06640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.73046875" bestFit="1" customWidth="1"/>
   </cols>
@@ -493,12 +499,21 @@
         <v>11</v>
       </c>
     </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{CFF59CB1-5500-4F10-A705-B9374BEF4C9F}"/>
     <hyperlink ref="B3" r:id="rId2" xr:uid="{E56C7ECF-6286-4ABE-B959-11D360773DEB}"/>
     <hyperlink ref="B4" r:id="rId3" xr:uid="{AEB2A04B-2B43-432E-BD45-CDC21EB05396}"/>
     <hyperlink ref="B5" r:id="rId4" xr:uid="{E5C8037E-8AC0-4156-B2B6-8CB87DEB7C4F}"/>
+    <hyperlink ref="B6" r:id="rId5" xr:uid="{C1BA6A99-37F0-4BF9-994D-622006E2BEC0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>